<commit_message>
Week 7 results + name changes
</commit_message>
<xml_diff>
--- a/FFL_Data.xlsx
+++ b/FFL_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edenaxelrad/Desktop/FFL-Dash-2025-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelrade\Downloads\FFL-Dash-2025-main\FFL-Dash-2025-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4112ABC-21F6-0D49-B0E9-CA533DF15492}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427EE618-916E-4ED7-98CA-6670AEB74EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1440" windowWidth="13920" windowHeight="11640" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
+    <workbookView xWindow="510" yWindow="3630" windowWidth="21600" windowHeight="11295" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Results" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="36">
   <si>
     <t>Points Against</t>
   </si>
@@ -84,12 +84,6 @@
     <t>The Legend of Drewkeys</t>
   </si>
   <si>
-    <t>You Gotta Gibbs!</t>
-  </si>
-  <si>
-    <t>Show Me the Mooney</t>
-  </si>
-  <si>
     <t>Bucky Charms</t>
   </si>
   <si>
@@ -133,6 +127,15 @@
   </si>
   <si>
     <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Golden Knights</t>
+  </si>
+  <si>
+    <t>Moonies of Io</t>
   </si>
 </sst>
 </file>
@@ -201,9 +204,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,7 +244,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -347,7 +350,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -489,7 +492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,19 +503,19 @@
   <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -529,7 +532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -543,7 +546,7 @@
         <v>124.56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -557,7 +560,7 @@
         <v>76.12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -571,7 +574,7 @@
         <v>108.82</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -585,7 +588,7 @@
         <v>101.22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -599,9 +602,9 @@
         <v>56.94</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -613,9 +616,9 @@
         <v>122.52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -627,9 +630,9 @@
         <v>101.88</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -641,9 +644,9 @@
         <v>87.38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -655,9 +658,9 @@
         <v>120.96</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -669,7 +672,7 @@
         <v>93.52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -683,7 +686,7 @@
         <v>102.6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -697,7 +700,7 @@
         <v>99.48</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -711,7 +714,7 @@
         <v>93.72</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -725,7 +728,7 @@
         <v>84.8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -739,7 +742,7 @@
         <v>128.44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -753,7 +756,7 @@
         <v>109.18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -767,9 +770,9 @@
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -781,9 +784,9 @@
         <v>92.18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -795,9 +798,9 @@
         <v>99.82</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -809,9 +812,9 @@
         <v>113.58</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -823,9 +826,9 @@
         <v>108.84</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -837,7 +840,7 @@
         <v>85.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -851,7 +854,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -865,7 +868,7 @@
         <v>91.88</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -879,7 +882,7 @@
         <v>87.38</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -893,7 +896,7 @@
         <v>137.52000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -907,7 +910,7 @@
         <v>102.52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -921,7 +924,7 @@
         <v>120.64</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -935,9 +938,9 @@
         <v>89.54</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -949,9 +952,9 @@
         <v>64.260000000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -963,9 +966,9 @@
         <v>101.82</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -977,9 +980,9 @@
         <v>112.2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -991,9 +994,9 @@
         <v>133.18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -1005,7 +1008,7 @@
         <v>99.12</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>82.72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1033,12 +1036,12 @@
         <v>111.32</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C38">
         <v>129.96</v>
@@ -1047,12 +1050,12 @@
         <v>126.18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C39">
         <v>120.58</v>
@@ -1061,12 +1064,12 @@
         <v>101.46</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C40">
         <v>93.3</v>
@@ -1075,12 +1078,12 @@
         <v>94.72</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C41">
         <v>150.12</v>
@@ -1089,12 +1092,12 @@
         <v>98.74</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C42">
         <v>100.6</v>
@@ -1103,12 +1106,12 @@
         <v>118.88</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C43">
         <v>98.74</v>
@@ -1117,12 +1120,12 @@
         <v>150.12</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44">
         <v>126.18</v>
@@ -1131,12 +1134,12 @@
         <v>129.96</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C45">
         <v>165</v>
@@ -1145,12 +1148,12 @@
         <v>92.48</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C46">
         <v>94.72</v>
@@ -1159,12 +1162,12 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C47">
         <v>101.46</v>
@@ -1173,12 +1176,12 @@
         <v>120.58</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C48">
         <v>118.88</v>
@@ -1187,12 +1190,12 @@
         <v>100.6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C49">
         <v>92.48</v>
@@ -1201,12 +1204,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C50">
         <v>92.98</v>
@@ -1215,12 +1218,12 @@
         <v>139.82</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C51">
         <v>153.08000000000001</v>
@@ -1229,12 +1232,12 @@
         <v>102.56</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C52">
         <v>139.82</v>
@@ -1243,12 +1246,12 @@
         <v>92.98</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C53">
         <v>97.34</v>
@@ -1257,12 +1260,12 @@
         <v>102.22</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C54">
         <v>102.56</v>
@@ -1271,12 +1274,12 @@
         <v>153.08000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55">
         <v>108.38</v>
@@ -1285,12 +1288,12 @@
         <v>109.5</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C56">
         <v>125.02</v>
@@ -1299,12 +1302,12 @@
         <v>94.46</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C57">
         <v>109.5</v>
@@ -1313,12 +1316,12 @@
         <v>108.38</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C58">
         <v>102.22</v>
@@ -1327,12 +1330,12 @@
         <v>97.34</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C59">
         <v>96.72</v>
@@ -1341,12 +1344,12 @@
         <v>97.38</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C60">
         <v>94.46</v>
@@ -1355,12 +1358,12 @@
         <v>125.02</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C61">
         <v>97.38</v>
@@ -1369,12 +1372,12 @@
         <v>96.72</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C62">
         <v>82.84</v>
@@ -1382,16 +1385,13 @@
       <c r="D62">
         <v>118.06</v>
       </c>
-      <c r="E62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C63">
         <v>74.58</v>
@@ -1399,16 +1399,13 @@
       <c r="D63">
         <v>63.1</v>
       </c>
-      <c r="E63" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C64">
         <v>128.4</v>
@@ -1416,16 +1413,13 @@
       <c r="D64">
         <v>99.64</v>
       </c>
-      <c r="E64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C65">
         <v>118.06</v>
@@ -1433,16 +1427,13 @@
       <c r="D65">
         <v>82.84</v>
       </c>
-      <c r="E65" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C66">
         <v>89.74</v>
@@ -1450,16 +1441,13 @@
       <c r="D66">
         <v>105</v>
       </c>
-      <c r="E66" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C67">
         <v>104.76</v>
@@ -1467,16 +1455,13 @@
       <c r="D67">
         <v>112.28</v>
       </c>
-      <c r="E67" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B68" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C68">
         <v>63.1</v>
@@ -1484,16 +1469,13 @@
       <c r="D68">
         <v>74.58</v>
       </c>
-      <c r="E68" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C69">
         <v>83.32</v>
@@ -1501,16 +1483,13 @@
       <c r="D69">
         <v>140.74</v>
       </c>
-      <c r="E69" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C70">
         <v>140.74</v>
@@ -1518,16 +1497,13 @@
       <c r="D70">
         <v>83.32</v>
       </c>
-      <c r="E70" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C71">
         <v>105</v>
@@ -1535,16 +1511,13 @@
       <c r="D71">
         <v>89.74</v>
       </c>
-      <c r="E71" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C72">
         <v>99.64</v>
@@ -1552,16 +1525,13 @@
       <c r="D72">
         <v>128.4</v>
       </c>
-      <c r="E72" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C73">
         <v>112.28</v>
@@ -1569,296 +1539,494 @@
       <c r="D73">
         <v>104.76</v>
       </c>
-      <c r="E73" t="s">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74">
+        <v>68.959999999999994</v>
+      </c>
+      <c r="D74">
+        <v>115.64</v>
+      </c>
+      <c r="E74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75">
+        <v>186.52</v>
+      </c>
+      <c r="D75">
+        <v>88.24</v>
+      </c>
+      <c r="E75" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>15</v>
+      </c>
+      <c r="B76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76">
+        <v>88.24</v>
+      </c>
+      <c r="D76">
+        <v>186.52</v>
+      </c>
+      <c r="E76" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B77" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77">
+        <v>83.3</v>
+      </c>
+      <c r="D77">
+        <v>67.22</v>
+      </c>
+      <c r="E77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78">
+        <v>71.540000000000006</v>
+      </c>
+      <c r="D78">
+        <v>81.180000000000007</v>
+      </c>
+      <c r="E78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79">
+        <v>166.86</v>
+      </c>
+      <c r="D79">
+        <v>114.18</v>
+      </c>
+      <c r="E79" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" t="s">
+        <v>33</v>
+      </c>
+      <c r="C80">
+        <v>131.74</v>
+      </c>
+      <c r="D80">
+        <v>80.92</v>
+      </c>
+      <c r="E80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" t="s">
+        <v>33</v>
+      </c>
+      <c r="C81">
+        <v>115.64</v>
+      </c>
+      <c r="D81">
+        <v>68.959999999999994</v>
+      </c>
+      <c r="E81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82">
+        <v>114.18</v>
+      </c>
+      <c r="D82">
+        <v>166.86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83">
+        <v>80.92</v>
+      </c>
+      <c r="D83">
+        <v>131.74</v>
+      </c>
+      <c r="E83" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84">
+        <v>67.22</v>
+      </c>
+      <c r="D84">
+        <v>83.3</v>
+      </c>
+      <c r="E84" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85">
+        <v>81.180000000000007</v>
+      </c>
+      <c r="D85">
+        <v>71.540000000000006</v>
+      </c>
+      <c r="E85" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C98" s="1"/>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C99" s="1"/>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C100" s="1"/>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{657FD601-2028-0A4F-BA12-553C96356FC4}">
-    <sortState ref="A2:E73">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E73">
       <sortCondition ref="B1:B73"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A151:A162">
-    <sortCondition ref="A151:A162"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C90:C101">
+    <sortCondition ref="C90:C101"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>